<commit_message>
New data (2 artices added)
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chapter_overbeck\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chapter_overbeck\mammals_book\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67674D7-D72A-4CE9-8A7B-89FB2FE4E23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C57CC9B-D8DD-4785-9AC5-766075D34CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="1029">
   <si>
     <t>Authors</t>
   </si>
@@ -3664,6 +3664,156 @@
   <si>
     <t>The species composition of rodents was studied from August 1992 to August 1993 and from February 1997 to March 1999 in areas of mixed forest with conifers and grasslands at Floresta Nacional de Sao Francisco de Paula (29º23'S, 50°23'W) and Centro de Pesquisas e Conservção da Natureza Pro-Mata (between 29"27' and 29º35'S, 50'08' and 50°15'W), Rio Grande do Sul State, southern Brazil. The small rodents were collected using Sherman live traps and pitfall traps. The larger ones were not captured but just recorded by visual identification or photo and film record. The study also presents a description of the vegetational community for that areas of intensive trapping effort. Thirteen species of rodents were identified: Akodon azarae. Akodon montensis, Lundomys molitor, Delomys dorsalis, Oligoryzomys flavescens, Oligoryzomys nigripes, Oryzomys ratticeps, Oxymycterus iheringi, Oxymycterus nasutus, Sphigurus villosus, Dasyprocta azarae, Phyllomys dasytrix, Kannabateomys amblyonix. Furthermore, the vegetal species Matayba cristae Keitz is registerecl for the first time in Rio Grande do Sul State.</t>
   </si>
+  <si>
+    <t>Stutz, NS; Hadler, P; Cherem, JJ; Pardinas, UFJ</t>
+  </si>
+  <si>
+    <t>Small mammal diversity in Semi-deciduous Seasonal Forest of the southernmost Brazilian Pampa: the importance of owl pellets for rapid inventories in human-changing ecosystems</t>
+  </si>
+  <si>
+    <t>ALL8</t>
+  </si>
+  <si>
+    <t>Papeis Avulsos de Zoologia</t>
+  </si>
+  <si>
+    <t>The Pampa biogeographic province covers a mere 2% of the Brazilian territory (176,496 km²). However, it stands out as a complex and diverse ecosystem, although its mammal communities are still scarcely understood. Human activities are transforming the territory into a mosaic of agroecosystems, native and exotic forest fragments, and grasslands. Here we conducted the first investigation to determine the richness of small mammal assemblages in the region based on extensive analyses of owl pellets (Tyto furcata). Craniodental remains were studied from samples collected from 12 Semi-deciduous Seasonal Forest sites in the municipality of São Lourenço do Sul, State of Rio Grande do Sul, Southern Brazil. A total of 2,617 individuals belonging to 18 taxa were recorded, including 2 marsupials (Didelphidae; 0.42%), 2 chiropterans (Molossidae, Phyllostomidae; 0.12%), and 14 rodents (Cricetidae, Muridae, Caviidae; 99.46%). The rodent genera Oligoryzomys, Mus, Calomys, and Akodon were the most common taxa. Large samples also included poorly known taxa, such as the cricetids Bibimys, Juliomys (recording here its southernmost occurrence), Lundomys, and Wilfredomys. From a biogeographical point of view, the recorded assemblage embraces a mixture of Platan, Pampean, and Atlantic Forest elements, highlighting the role of the southernmost Brazilian hills as a wedge favoring the penetration of forest micromammals to higher latitudes. Our findings testify to the great diversity of the Pampa, but also point to a growing homogeneity and dominance of rodent species that are widespread in agroecosystems. Rapid inventories based on owl pellets emerge as a suitable, economic, non-invasive tool to document these community changes.</t>
+  </si>
+  <si>
+    <t>e20206025</t>
+  </si>
+  <si>
+    <t>10.11606/1807-0205/2020.60.25</t>
+  </si>
+  <si>
+    <t>Boa Vista I</t>
+  </si>
+  <si>
+    <t>Boa Vista II</t>
+  </si>
+  <si>
+    <t>Boqueirão</t>
+  </si>
+  <si>
+    <t>Canta Galo</t>
+  </si>
+  <si>
+    <t>Evaristo I</t>
+  </si>
+  <si>
+    <t>Evaristo II</t>
+  </si>
+  <si>
+    <t>Picada das Antas</t>
+  </si>
+  <si>
+    <t>Picada Feliz I</t>
+  </si>
+  <si>
+    <t>Picada Feliz II</t>
+  </si>
+  <si>
+    <t>Quevedos I</t>
+  </si>
+  <si>
+    <t>Quevedos II</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>31°15′17″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°12′31″W</t>
+  </si>
+  <si>
+    <t>31°15′18″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°12′34″W</t>
+  </si>
+  <si>
+    <t>31°16′55″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°04′39″W</t>
+  </si>
+  <si>
+    <t>31°10′58″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°21′19″W</t>
+  </si>
+  <si>
+    <t>31°11′13″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°13′58″W</t>
+  </si>
+  <si>
+    <t>31°10′43″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°18′25″W</t>
+  </si>
+  <si>
+    <t>31°18′48″S</t>
+  </si>
+  <si>
+    <t>31°12′39″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°15′29″W</t>
+  </si>
+  <si>
+    <t>31°12′46″S</t>
+  </si>
+  <si>
+    <t>31°14′41″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°15′35″W</t>
+  </si>
+  <si>
+    <t>31°13′51″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°14′37″W</t>
+  </si>
+  <si>
+    <t>31°17′47″S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52°09′38″W</t>
+  </si>
+  <si>
+    <t>ALL9</t>
+  </si>
+  <si>
+    <t>Santos, TM, Spies, MR, Koop, K, Trevisan, R, Cechin, SZ</t>
+  </si>
+  <si>
+    <t>Mammals of the campus of the Universidade Federal de Santa Maria, Rio Grande do Sul, Brazil.</t>
+  </si>
+  <si>
+    <t>The study was conducted in the Campus of the Universidade Federal de Santa Maria (UFSM), which is located in the Central Depression of Rio Grande do Sul State, in the Pampa biome. Here, a mammal list is presented and spatial occupation and conservation strategies of local mammals are discussed. Between November 2001 and October 2002, 26 native species and two exotic species of mammals (Lepus europaeus and Mus musculus) were recorded, representing 14 families. Most recorded species presents wide distribution, is likely associated to open environments and is tolerant to human disturbances. However, we also recorded three species that are considered rare or threatened in the State of Rio Grande do Sul (Lontra longicaudis, Monodelphis dimidiata and Nyctinomops laticaudatus), for which conservation strategies are recommended. The low species richness recorded in the Campus can be related to the strong pressure of human disturbances, to the small extension of the studied area or to historical factors, as the studied area is originally a grassland (Pampa), a type of environment containing a lower mammalian diversity than native forests.</t>
+  </si>
+  <si>
+    <t>Campus da Universidade Federal de Santa Maria (UFSM),</t>
+  </si>
+  <si>
+    <t>53° 42’ W</t>
+  </si>
+  <si>
+    <t>29° 42’ S</t>
+  </si>
+  <si>
+    <t>jan/mar</t>
+  </si>
+  <si>
+    <t>10.1590/S1676-06032008000100015  </t>
+  </si>
 </sst>
 </file>
 
@@ -3818,7 +3968,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -3845,6 +3995,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -4127,13 +4278,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA190"/>
+  <dimension ref="A1:AA203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F159" sqref="F159"/>
+      <selection pane="bottomRight" activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14836,2147 +14987,2980 @@
         <v>-50.383333</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G156" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H156" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I156" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K156" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L156" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M156" t="s">
+        <v>984</v>
+      </c>
+      <c r="N156" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O156" t="s">
+        <v>986</v>
+      </c>
+      <c r="P156" t="s">
+        <v>998</v>
+      </c>
+      <c r="Q156" s="8" t="s">
+        <v>999</v>
+      </c>
+      <c r="R156" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S156" s="1"/>
+      <c r="T156" s="3">
+        <v>-31.254722000000001</v>
+      </c>
+      <c r="U156" s="3">
+        <v>-52.208610999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G157" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H157" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I157" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K157" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L157" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M157" t="s">
+        <v>984</v>
+      </c>
+      <c r="N157" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O157" t="s">
+        <v>987</v>
+      </c>
+      <c r="P157" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Q157" s="8" t="s">
+        <v>1001</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S157" s="1"/>
+      <c r="T157" s="3">
+        <v>-31.254992999999999</v>
+      </c>
+      <c r="U157" s="3">
+        <v>-52.209425000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G158" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H158" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I158" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K158" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L158" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M158" t="s">
+        <v>984</v>
+      </c>
+      <c r="N158" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O158" t="s">
+        <v>988</v>
+      </c>
+      <c r="P158" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Q158" s="8" t="s">
+        <v>1003</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S158" s="1"/>
+      <c r="T158" s="3">
+        <v>-31.281943999999999</v>
+      </c>
+      <c r="U158" s="3">
+        <v>-52.077503</v>
+      </c>
+    </row>
+    <row r="159" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G159" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H159" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I159" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K159" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L159" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M159" t="s">
+        <v>984</v>
+      </c>
+      <c r="N159" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O159" t="s">
+        <v>989</v>
+      </c>
+      <c r="P159" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Q159" s="8" t="s">
+        <v>1005</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S159" s="1"/>
+      <c r="T159" s="3">
+        <v>-31.182779</v>
+      </c>
+      <c r="U159" s="3">
+        <v>-52.355274000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G160" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H160" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I160" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K160" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L160" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M160" t="s">
+        <v>984</v>
+      </c>
+      <c r="N160" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O160" t="s">
+        <v>990</v>
+      </c>
+      <c r="P160" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Q160" s="8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S160" s="1"/>
+      <c r="T160" s="3">
+        <v>-31.186944</v>
+      </c>
+      <c r="U160" s="3">
+        <v>-52.232785999999997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G161" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H161" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I161" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K161" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L161" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M161" t="s">
+        <v>984</v>
+      </c>
+      <c r="N161" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O161" t="s">
+        <v>991</v>
+      </c>
+      <c r="P161" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q161" s="8" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R161" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S161" s="1"/>
+      <c r="T161" s="3">
+        <v>-31.178612000000001</v>
+      </c>
+      <c r="U161" s="3">
+        <v>-52.306935000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G162" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H162" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I162" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K162" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L162" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M162" t="s">
+        <v>984</v>
+      </c>
+      <c r="N162" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O162" t="s">
+        <v>992</v>
+      </c>
+      <c r="P162" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q162" s="8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S162" s="1"/>
+      <c r="T162" s="3">
+        <v>-31.313331999999999</v>
+      </c>
+      <c r="U162" s="3">
+        <v>-52.232779000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G163" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H163" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I163" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K163" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L163" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M163" t="s">
+        <v>984</v>
+      </c>
+      <c r="N163" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O163" t="s">
+        <v>993</v>
+      </c>
+      <c r="P163" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Q163" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S163" s="1"/>
+      <c r="T163" s="3">
+        <v>-31.210861000000001</v>
+      </c>
+      <c r="U163" s="3">
+        <v>-52.258111999999997</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G164" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H164" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I164" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K164" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L164" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M164" t="s">
+        <v>984</v>
+      </c>
+      <c r="N164" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O164" t="s">
+        <v>994</v>
+      </c>
+      <c r="P164" t="s">
+        <v>1013</v>
+      </c>
+      <c r="Q164" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S164" s="1"/>
+      <c r="T164" s="3">
+        <v>-31.212778</v>
+      </c>
+      <c r="U164" s="3">
+        <v>-52.258056000000003</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G165" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H165" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I165" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K165" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L165" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M165" t="s">
+        <v>984</v>
+      </c>
+      <c r="N165" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O165" t="s">
+        <v>995</v>
+      </c>
+      <c r="P165" t="s">
+        <v>1014</v>
+      </c>
+      <c r="Q165" s="8" t="s">
+        <v>1015</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S165" s="1"/>
+      <c r="T165" s="3">
+        <v>-31.244713000000001</v>
+      </c>
+      <c r="U165" s="3">
+        <v>-52.259721999999996</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G166" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H166" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I166" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K166" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L166" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M166" t="s">
+        <v>984</v>
+      </c>
+      <c r="N166" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O166" t="s">
+        <v>996</v>
+      </c>
+      <c r="P166" t="s">
+        <v>1016</v>
+      </c>
+      <c r="Q166" s="8" t="s">
+        <v>1017</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S166" s="1"/>
+      <c r="T166" s="3">
+        <v>-31.230837000000001</v>
+      </c>
+      <c r="U166" s="3">
+        <v>-52.243614999999998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="G167" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H167" s="3">
+        <f>2020</f>
+        <v>2020</v>
+      </c>
+      <c r="I167" s="3">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K167" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="L167" s="3">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="M167" t="s">
+        <v>984</v>
+      </c>
+      <c r="N167" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="O167" t="s">
+        <v>997</v>
+      </c>
+      <c r="P167" t="s">
+        <v>1018</v>
+      </c>
+      <c r="Q167" s="8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="S167" s="1"/>
+      <c r="T167" s="3">
+        <v>-31.296386999999999</v>
+      </c>
+      <c r="U167" s="3">
+        <v>-52.160558000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G168" s="8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H168" s="3">
+        <f>2008</f>
+        <v>2008</v>
+      </c>
+      <c r="I168" s="3">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="J168" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="K168" s="3">
+        <f>125</f>
+        <v>125</v>
+      </c>
+      <c r="L168" s="3">
+        <f>131</f>
+        <v>131</v>
+      </c>
+      <c r="N168" s="20" t="s">
+        <v>1028</v>
+      </c>
+      <c r="O168" t="s">
+        <v>1024</v>
+      </c>
+      <c r="P168" t="s">
+        <v>1026</v>
+      </c>
+      <c r="Q168" t="s">
+        <v>1025</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="S168" s="1"/>
+      <c r="T168" s="3">
+        <v>-29.720516</v>
+      </c>
+      <c r="U168" s="3">
+        <v>-53.715730000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
         <v>813</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B169" s="3" t="s">
         <v>814</v>
       </c>
-      <c r="C156" s="3" t="s">
+      <c r="C169" s="3" t="s">
         <v>814</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D169" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E169" s="3" t="s">
         <v>815</v>
       </c>
-      <c r="F156" s="3" t="s">
+      <c r="F169" s="3" t="s">
         <v>816</v>
       </c>
-      <c r="G156" s="3" t="s">
+      <c r="G169" s="3" t="s">
         <v>817</v>
       </c>
-      <c r="H156" s="3">
+      <c r="H169" s="3">
         <v>2004</v>
       </c>
-      <c r="I156" s="3">
+      <c r="I169" s="3">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="J156" s="3">
+      <c r="J169" s="3">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="K156" s="3">
+      <c r="K169" s="3">
         <f>147</f>
         <v>147</v>
       </c>
-      <c r="L156" s="3">
+      <c r="L169" s="3">
         <f>167</f>
         <v>167</v>
       </c>
-      <c r="O156" s="3" t="s">
+      <c r="O169" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="P156" s="8" t="s">
+      <c r="P169" s="8" t="s">
         <v>904</v>
       </c>
-      <c r="Q156" s="8" t="s">
+      <c r="Q169" s="8" t="s">
         <v>905</v>
       </c>
-      <c r="R156" s="1" t="s">
+      <c r="R169" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="T156" s="3">
+      <c r="T169" s="3">
         <v>-29.383333</v>
       </c>
-      <c r="U156" s="3">
+      <c r="U169" s="3">
         <v>-50.383333</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A157" s="3" t="s">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B170" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C170" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E170" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="F157" s="10" t="s">
+      <c r="F170" s="10" t="s">
         <v>978</v>
       </c>
-      <c r="G157" s="3" t="s">
+      <c r="G170" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="H157" s="3">
+      <c r="H170" s="3">
         <f>2002</f>
         <v>2002</v>
       </c>
-      <c r="I157" s="3">
+      <c r="I170" s="3">
         <f>15</f>
         <v>15</v>
       </c>
-      <c r="J157" s="3">
+      <c r="J170" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K157" s="3">
+      <c r="K170" s="3">
         <f>61</f>
         <v>61</v>
       </c>
-      <c r="L157" s="3">
+      <c r="L170" s="3">
         <f>86</f>
         <v>86</v>
       </c>
-      <c r="O157" s="3" t="s">
+      <c r="O170" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="P157" s="8" t="s">
+      <c r="P170" s="8" t="s">
         <v>904</v>
       </c>
-      <c r="Q157" s="8" t="s">
+      <c r="Q170" s="8" t="s">
         <v>905</v>
       </c>
-      <c r="R157" s="1" t="s">
+      <c r="R170" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="T157" s="3">
+      <c r="T170" s="3">
         <v>-29.383333</v>
       </c>
-      <c r="U157" s="3">
+      <c r="U170" s="3">
         <v>-50.383333</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A158" s="3" t="s">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B171" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C171" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D171" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E171" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="F158" s="10" t="s">
+      <c r="F171" s="10" t="s">
         <v>978</v>
       </c>
-      <c r="G158" s="3" t="s">
+      <c r="G171" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="H158" s="3">
+      <c r="H171" s="3">
         <f>2002</f>
         <v>2002</v>
       </c>
-      <c r="I158" s="3">
+      <c r="I171" s="3">
         <f>15</f>
         <v>15</v>
       </c>
-      <c r="J158" s="3">
+      <c r="J171" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K158" s="3">
+      <c r="K171" s="3">
         <f>61</f>
         <v>61</v>
       </c>
-      <c r="L158" s="3">
+      <c r="L171" s="3">
         <f>86</f>
         <v>86</v>
       </c>
-      <c r="O158" s="3" t="s">
+      <c r="O171" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="P158" s="8" t="s">
+      <c r="P171" s="8" t="s">
         <v>907</v>
       </c>
-      <c r="Q158" s="8" t="s">
+      <c r="Q171" s="8" t="s">
         <v>908</v>
       </c>
-      <c r="R158" s="1" t="s">
+      <c r="R171" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S158" s="3" t="s">
+      <c r="S171" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T158" s="3">
+      <c r="T171" s="3">
         <v>-29.583687999999999</v>
       </c>
-      <c r="U158" s="3">
+      <c r="U171" s="3">
         <v>-50.249971000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A159" s="3" t="s">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B172" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C172" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D172" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E172" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="F159" s="10" t="s">
+      <c r="F172" s="10" t="s">
         <v>978</v>
       </c>
-      <c r="G159" s="3" t="s">
+      <c r="G172" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="H159" s="3">
+      <c r="H172" s="3">
         <f>2002</f>
         <v>2002</v>
       </c>
-      <c r="I159" s="3">
+      <c r="I172" s="3">
         <f>15</f>
         <v>15</v>
       </c>
-      <c r="J159" s="3">
+      <c r="J172" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K159" s="3">
+      <c r="K172" s="3">
         <f>61</f>
         <v>61</v>
       </c>
-      <c r="L159" s="3">
+      <c r="L172" s="3">
         <f>86</f>
         <v>86</v>
       </c>
-      <c r="O159" s="3" t="s">
+      <c r="O172" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="P159" s="8" t="s">
+      <c r="P172" s="8" t="s">
         <v>910</v>
       </c>
-      <c r="Q159" s="8" t="s">
+      <c r="Q172" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="R159" s="1" t="s">
+      <c r="R172" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S159" s="3" t="s">
+      <c r="S172" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T159" s="3">
+      <c r="T172" s="3">
         <v>-29.45</v>
       </c>
-      <c r="U159" s="3">
+      <c r="U172" s="3">
         <v>-50.133333</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A160" s="3" t="s">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="B173" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C173" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D173" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E173" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F160" s="3" t="s">
+      <c r="F173" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="G160" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="H160" s="3">
+      <c r="G173" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H173" s="3">
         <f>2015</f>
         <v>2015</v>
       </c>
-      <c r="I160" s="3">
+      <c r="I173" s="3">
         <v>73</v>
       </c>
-      <c r="K160" s="3">
+      <c r="K173" s="3">
         <f>42</f>
         <v>42</v>
       </c>
-      <c r="L160" s="3">
+      <c r="L173" s="3">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="O160" s="3" t="s">
+      <c r="O173" s="3" t="s">
         <v>913</v>
       </c>
-      <c r="P160" s="17" t="s">
+      <c r="P173" s="17" t="s">
         <v>915</v>
       </c>
-      <c r="Q160" s="17" t="s">
+      <c r="Q173" s="17" t="s">
         <v>916</v>
       </c>
-      <c r="R160" s="1" t="s">
+      <c r="R173" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T160" s="3">
+      <c r="T173" s="3">
         <v>-26.568856</v>
       </c>
-      <c r="U160" s="3">
+      <c r="U173" s="3">
         <v>-51.671531000000002</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A161" s="3" t="s">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B174" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C174" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="E174" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F161" s="3" t="s">
+      <c r="F174" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="G161" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="H161" s="3">
+      <c r="G174" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H174" s="3">
         <f>2015</f>
         <v>2015</v>
       </c>
-      <c r="I161" s="3">
+      <c r="I174" s="3">
         <v>73</v>
       </c>
-      <c r="K161" s="3">
+      <c r="K174" s="3">
         <f>42</f>
         <v>42</v>
       </c>
-      <c r="L161" s="3">
+      <c r="L174" s="3">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="O161" s="3" t="s">
+      <c r="O174" s="3" t="s">
         <v>914</v>
       </c>
-      <c r="P161" s="17" t="s">
+      <c r="P174" s="17" t="s">
         <v>917</v>
       </c>
-      <c r="Q161" s="17" t="s">
+      <c r="Q174" s="17" t="s">
         <v>918</v>
       </c>
-      <c r="R161" s="1" t="s">
+      <c r="R174" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T161" s="3">
+      <c r="T174" s="3">
         <v>-26.581365999999999</v>
       </c>
-      <c r="U161" s="3">
+      <c r="U174" s="3">
         <v>-51.712150999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A162" s="3" t="s">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
         <v>832</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B175" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C175" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="D162" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>834</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E175" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F162" s="3" t="s">
+      <c r="F175" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="G162" s="3" t="s">
+      <c r="G175" s="3" t="s">
         <v>838</v>
       </c>
-      <c r="H162" s="3">
+      <c r="H175" s="3">
         <f>2016</f>
         <v>2016</v>
       </c>
-      <c r="I162" s="12">
+      <c r="I175" s="12">
         <v>97</v>
       </c>
-      <c r="J162" s="12">
+      <c r="J175" s="12">
         <v>5</v>
       </c>
-      <c r="K162" s="3">
+      <c r="K175" s="3">
         <v>1469</v>
       </c>
-      <c r="L162" s="3">
+      <c r="L175" s="3">
         <v>1482</v>
       </c>
-      <c r="N162" s="3" t="s">
+      <c r="N175" s="3" t="s">
         <v>837</v>
       </c>
-      <c r="O162" s="3" t="s">
+      <c r="O175" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="P162" s="17" t="s">
+      <c r="P175" s="17" t="s">
         <v>961</v>
       </c>
-      <c r="Q162" s="17" t="s">
+      <c r="Q175" s="17" t="s">
         <v>962</v>
       </c>
-      <c r="R162" s="1" t="s">
+      <c r="R175" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T162" s="3">
+      <c r="T175" s="3">
         <v>-29.159993</v>
       </c>
-      <c r="U162" s="3">
+      <c r="U175" s="3">
         <v>-50.100005000000003</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A163" s="3" t="s">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B176" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C176" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D163" s="3" t="s">
+      <c r="D176" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E176" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F163" s="3" t="s">
+      <c r="F176" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G163" s="3" t="s">
+      <c r="G176" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H163" s="3">
+      <c r="H176" s="3">
         <v>2012</v>
       </c>
-      <c r="I163" s="12">
+      <c r="I176" s="12">
         <v>93</v>
       </c>
-      <c r="J163" s="12">
+      <c r="J176" s="12">
         <v>5</v>
       </c>
-      <c r="K163" s="12">
+      <c r="K176" s="12">
         <v>1355</v>
       </c>
-      <c r="L163" s="3">
+      <c r="L176" s="3">
         <v>1367</v>
       </c>
-      <c r="N163" s="3" t="s">
+      <c r="N176" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O163" s="17" t="s">
+      <c r="O176" s="17" t="s">
         <v>919</v>
       </c>
-      <c r="P163" s="3" t="s">
+      <c r="P176" s="3" t="s">
         <v>921</v>
       </c>
-      <c r="Q163" s="17" t="s">
+      <c r="Q176" s="17" t="s">
         <v>967</v>
       </c>
-      <c r="R163" s="1" t="s">
+      <c r="R176" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T163" s="3">
+      <c r="T176" s="3">
         <v>-29.393318000000001</v>
       </c>
-      <c r="U163" s="3">
+      <c r="U176" s="3">
         <v>-55.429262000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A164" s="3" t="s">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A177" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B177" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C164" s="3" t="s">
+      <c r="C177" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D164" s="3" t="s">
+      <c r="D177" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E177" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F164" s="3" t="s">
+      <c r="F177" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G164" s="3" t="s">
+      <c r="G177" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H164" s="3">
+      <c r="H177" s="3">
         <v>2012</v>
       </c>
-      <c r="I164" s="12">
+      <c r="I177" s="12">
         <v>93</v>
       </c>
-      <c r="J164" s="12">
+      <c r="J177" s="12">
         <v>5</v>
       </c>
-      <c r="K164" s="12">
+      <c r="K177" s="12">
         <v>1355</v>
       </c>
-      <c r="L164" s="3">
+      <c r="L177" s="3">
         <v>1367</v>
       </c>
-      <c r="N164" s="3" t="s">
+      <c r="N177" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O164" s="17" t="s">
+      <c r="O177" s="17" t="s">
         <v>919</v>
       </c>
-      <c r="P164" s="17" t="s">
+      <c r="P177" s="17" t="s">
         <v>968</v>
       </c>
-      <c r="Q164" s="17" t="s">
+      <c r="Q177" s="17" t="s">
         <v>969</v>
       </c>
-      <c r="R164" s="1" t="s">
+      <c r="R177" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T164" s="3">
+      <c r="T177" s="3">
         <v>-29.403306000000001</v>
       </c>
-      <c r="U164" s="3">
+      <c r="U177" s="3">
         <v>-55.580278</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A165" s="3" t="s">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B178" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C165" s="3" t="s">
+      <c r="C178" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="D178" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="E178" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F165" s="3" t="s">
+      <c r="F178" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G165" s="3" t="s">
+      <c r="G178" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H165" s="3">
+      <c r="H178" s="3">
         <v>2012</v>
       </c>
-      <c r="I165" s="12">
+      <c r="I178" s="12">
         <v>93</v>
       </c>
-      <c r="J165" s="12">
+      <c r="J178" s="12">
         <v>5</v>
       </c>
-      <c r="K165" s="12">
+      <c r="K178" s="12">
         <v>1355</v>
       </c>
-      <c r="L165" s="3">
+      <c r="L178" s="3">
         <v>1367</v>
       </c>
-      <c r="N165" s="3" t="s">
+      <c r="N178" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O165" s="17" t="s">
+      <c r="O178" s="17" t="s">
         <v>919</v>
       </c>
-      <c r="P165" s="17" t="s">
+      <c r="P178" s="17" t="s">
         <v>970</v>
       </c>
-      <c r="Q165" s="17" t="s">
+      <c r="Q178" s="17" t="s">
         <v>971</v>
       </c>
-      <c r="R165" s="1" t="s">
+      <c r="R178" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T165" s="3">
+      <c r="T178" s="3">
         <v>-29.321805999999999</v>
       </c>
-      <c r="U165" s="3">
+      <c r="U178" s="3">
         <v>-55.536332999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A166" s="3" t="s">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A179" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B179" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C166" s="3" t="s">
+      <c r="C179" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D166" s="3" t="s">
+      <c r="D179" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E166" s="3" t="s">
+      <c r="E179" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F166" s="3" t="s">
+      <c r="F179" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G166" s="3" t="s">
+      <c r="G179" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H166" s="3">
+      <c r="H179" s="3">
         <v>2012</v>
       </c>
-      <c r="I166" s="12">
+      <c r="I179" s="12">
         <v>93</v>
       </c>
-      <c r="J166" s="12">
+      <c r="J179" s="12">
         <v>5</v>
       </c>
-      <c r="K166" s="12">
+      <c r="K179" s="12">
         <v>1355</v>
       </c>
-      <c r="L166" s="3">
+      <c r="L179" s="3">
         <v>1367</v>
       </c>
-      <c r="N166" s="3" t="s">
+      <c r="N179" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O166" s="17" t="s">
+      <c r="O179" s="17" t="s">
         <v>919</v>
       </c>
-      <c r="P166" s="17" t="s">
+      <c r="P179" s="17" t="s">
         <v>972</v>
       </c>
-      <c r="Q166" s="17" t="s">
+      <c r="Q179" s="17" t="s">
         <v>973</v>
       </c>
-      <c r="R166" s="1" t="s">
+      <c r="R179" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T166" s="3">
+      <c r="T179" s="3">
         <v>-29.230733000000001</v>
       </c>
-      <c r="U166" s="3">
+      <c r="U179" s="3">
         <v>-55.467174999999997</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A167" s="3" t="s">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A180" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B180" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C180" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D180" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E167" s="3" t="s">
+      <c r="E180" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F167" s="3" t="s">
+      <c r="F180" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G167" s="3" t="s">
+      <c r="G180" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H167" s="3">
+      <c r="H180" s="3">
         <v>2012</v>
       </c>
-      <c r="I167" s="12">
+      <c r="I180" s="12">
         <v>93</v>
       </c>
-      <c r="J167" s="12">
+      <c r="J180" s="12">
         <v>5</v>
       </c>
-      <c r="K167" s="12">
+      <c r="K180" s="12">
         <v>1355</v>
       </c>
-      <c r="L167" s="3">
+      <c r="L180" s="3">
         <v>1367</v>
       </c>
-      <c r="N167" s="3" t="s">
+      <c r="N180" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O167" s="17" t="s">
+      <c r="O180" s="17" t="s">
         <v>920</v>
       </c>
-      <c r="P167" s="17" t="s">
+      <c r="P180" s="17" t="s">
         <v>974</v>
       </c>
-      <c r="Q167" s="17" t="s">
+      <c r="Q180" s="17" t="s">
         <v>975</v>
       </c>
-      <c r="R167" s="1" t="s">
+      <c r="R180" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T167" s="3">
+      <c r="T180" s="3">
         <v>-29.159614000000001</v>
       </c>
-      <c r="U167" s="3">
+      <c r="U180" s="3">
         <v>-55.421002000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A168" s="3" t="s">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A181" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B181" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="C181" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D181" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E168" s="3" t="s">
+      <c r="E181" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F168" s="3" t="s">
+      <c r="F181" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="G168" s="3" t="s">
+      <c r="G181" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H168" s="3">
+      <c r="H181" s="3">
         <v>2012</v>
       </c>
-      <c r="I168" s="12">
+      <c r="I181" s="12">
         <v>93</v>
       </c>
-      <c r="J168" s="12">
+      <c r="J181" s="12">
         <v>5</v>
       </c>
-      <c r="K168" s="12">
+      <c r="K181" s="12">
         <v>1355</v>
       </c>
-      <c r="L168" s="3">
+      <c r="L181" s="3">
         <v>1367</v>
       </c>
-      <c r="N168" s="3" t="s">
+      <c r="N181" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="O168" s="17" t="s">
+      <c r="O181" s="17" t="s">
         <v>920</v>
       </c>
-      <c r="P168" s="17" t="s">
+      <c r="P181" s="17" t="s">
         <v>976</v>
       </c>
-      <c r="Q168" s="17" t="s">
+      <c r="Q181" s="17" t="s">
         <v>977</v>
       </c>
-      <c r="R168" s="1" t="s">
+      <c r="R181" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T168" s="3">
+      <c r="T181" s="3">
         <v>-29.126294999999999</v>
       </c>
-      <c r="U168" s="3">
+      <c r="U181" s="3">
         <v>-55.399900000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A169" s="3" t="s">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A182" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B182" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="C182" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D182" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="E169" s="3" t="s">
+      <c r="E182" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F169" s="3" t="s">
+      <c r="F182" s="3" t="s">
         <v>849</v>
       </c>
-      <c r="G169" s="3" t="s">
+      <c r="G182" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="H169" s="12">
+      <c r="H182" s="12">
         <v>2007</v>
       </c>
-      <c r="I169" s="3">
+      <c r="I182" s="3">
         <v>88</v>
       </c>
-      <c r="J169" s="3">
+      <c r="J182" s="3">
         <v>3</v>
       </c>
-      <c r="K169" s="3">
+      <c r="K182" s="3">
         <v>769</v>
       </c>
-      <c r="L169" s="3">
+      <c r="L182" s="3">
         <v>776</v>
       </c>
-      <c r="N169" s="3" t="s">
+      <c r="N182" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="O169" s="3" t="s">
+      <c r="O182" s="3" t="s">
         <v>922</v>
       </c>
-      <c r="P169" s="19" t="s">
+      <c r="P182" s="19" t="s">
         <v>963</v>
       </c>
-      <c r="Q169" s="19" t="s">
+      <c r="Q182" s="19" t="s">
         <v>964</v>
       </c>
-      <c r="R169" s="1" t="s">
+      <c r="R182" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S169" s="3" t="s">
+      <c r="S182" s="3" t="s">
         <v>924</v>
       </c>
-      <c r="T169" s="3">
+      <c r="T182" s="3">
         <v>-32.504286</v>
       </c>
-      <c r="U169" s="3">
+      <c r="U182" s="3">
         <v>-52.576135000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A170" s="3" t="s">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A183" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B183" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C183" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D183" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="E170" s="3" t="s">
+      <c r="E183" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F170" s="3" t="s">
+      <c r="F183" s="3" t="s">
         <v>849</v>
       </c>
-      <c r="G170" s="3" t="s">
+      <c r="G183" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="H170" s="12">
+      <c r="H183" s="12">
         <v>2007</v>
       </c>
-      <c r="I170" s="3">
+      <c r="I183" s="3">
         <v>88</v>
       </c>
-      <c r="J170" s="3">
+      <c r="J183" s="3">
         <v>3</v>
       </c>
-      <c r="K170" s="3">
+      <c r="K183" s="3">
         <v>769</v>
       </c>
-      <c r="L170" s="3">
+      <c r="L183" s="3">
         <v>776</v>
       </c>
-      <c r="N170" s="3" t="s">
+      <c r="N183" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="O170" s="3" t="s">
+      <c r="O183" s="3" t="s">
         <v>923</v>
       </c>
-      <c r="P170" s="19" t="s">
+      <c r="P183" s="19" t="s">
         <v>771</v>
       </c>
-      <c r="Q170" s="19" t="s">
+      <c r="Q183" s="19" t="s">
         <v>965</v>
       </c>
-      <c r="R170" s="1" t="s">
+      <c r="R183" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S170" s="3" t="s">
+      <c r="S183" s="3" t="s">
         <v>924</v>
       </c>
-      <c r="T170" s="3">
+      <c r="T183" s="3">
         <v>-30.340088000000002</v>
       </c>
-      <c r="U170" s="3">
+      <c r="U183" s="3">
         <v>-50.270386000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A171" s="3" t="s">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A184" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="B171" s="3" t="s">
+      <c r="B184" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="C171" s="3" t="s">
+      <c r="C184" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="D171" s="3" t="s">
+      <c r="D184" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="E171" s="3" t="s">
+      <c r="E184" s="3" t="s">
         <v>853</v>
       </c>
-      <c r="F171" s="3" t="s">
+      <c r="F184" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="G171" s="3" t="s">
+      <c r="G184" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H171" s="3">
+      <c r="H184" s="3">
         <v>2011</v>
       </c>
-      <c r="I171" s="3">
+      <c r="I184" s="3">
         <v>9</v>
       </c>
-      <c r="J171" s="3">
+      <c r="J184" s="3">
         <v>3</v>
       </c>
-      <c r="K171" s="3">
+      <c r="K184" s="3">
         <v>278</v>
       </c>
-      <c r="L171" s="3">
+      <c r="L184" s="3">
         <v>288</v>
       </c>
-      <c r="O171" s="3" t="s">
+      <c r="O184" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="P171" s="8" t="s">
+      <c r="P184" s="8" t="s">
         <v>904</v>
       </c>
-      <c r="Q171" s="8" t="s">
+      <c r="Q184" s="8" t="s">
         <v>905</v>
       </c>
-      <c r="R171" s="1" t="s">
+      <c r="R184" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S171" s="3" t="s">
+      <c r="S184" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T171" s="3">
+      <c r="T184" s="3">
         <v>-29.383333</v>
       </c>
-      <c r="U171" s="3">
+      <c r="U184" s="3">
         <v>-50.383333</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A172" s="3" t="s">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A185" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B185" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="C172" s="3" t="s">
+      <c r="C185" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="D172" s="3" t="s">
+      <c r="D185" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="E172" s="3" t="s">
+      <c r="E185" s="3" t="s">
         <v>853</v>
       </c>
-      <c r="F172" s="3" t="s">
+      <c r="F185" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="G172" s="3" t="s">
+      <c r="G185" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H172" s="3">
+      <c r="H185" s="3">
         <v>2011</v>
       </c>
-      <c r="I172" s="3">
+      <c r="I185" s="3">
         <v>9</v>
       </c>
-      <c r="J172" s="3">
+      <c r="J185" s="3">
         <v>3</v>
       </c>
-      <c r="K172" s="3">
+      <c r="K185" s="3">
         <v>278</v>
       </c>
-      <c r="L172" s="3">
+      <c r="L185" s="3">
         <v>288</v>
       </c>
-      <c r="O172" s="3" t="s">
+      <c r="O185" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="P172" s="8" t="s">
+      <c r="P185" s="8" t="s">
         <v>925</v>
       </c>
-      <c r="Q172" s="8" t="s">
+      <c r="Q185" s="8" t="s">
         <v>926</v>
       </c>
-      <c r="R172" s="1" t="s">
+      <c r="R185" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S172" s="3" t="s">
+      <c r="S185" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T172" s="3">
+      <c r="T185" s="3">
         <v>-29.45</v>
       </c>
-      <c r="U172" s="3">
+      <c r="U185" s="3">
         <v>-50.416646</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A173" s="3" t="s">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A186" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B186" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="C173" s="3" t="s">
+      <c r="C186" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="D173" s="3" t="s">
+      <c r="D186" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="E173" s="3" t="s">
+      <c r="E186" s="3" t="s">
         <v>853</v>
       </c>
-      <c r="F173" s="3" t="s">
+      <c r="F186" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="G173" s="3" t="s">
+      <c r="G186" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H173" s="3">
+      <c r="H186" s="3">
         <v>2011</v>
       </c>
-      <c r="I173" s="3">
+      <c r="I186" s="3">
         <v>9</v>
       </c>
-      <c r="J173" s="3">
+      <c r="J186" s="3">
         <v>3</v>
       </c>
-      <c r="K173" s="3">
+      <c r="K186" s="3">
         <v>278</v>
       </c>
-      <c r="L173" s="3">
+      <c r="L186" s="3">
         <v>288</v>
       </c>
-      <c r="O173" s="3" t="s">
+      <c r="O186" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="P173" s="8" t="s">
+      <c r="P186" s="8" t="s">
         <v>927</v>
       </c>
-      <c r="Q173" s="8" t="s">
+      <c r="Q186" s="8" t="s">
         <v>908</v>
       </c>
-      <c r="R173" s="1" t="s">
+      <c r="R186" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S173" s="3" t="s">
+      <c r="S186" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T173" s="3">
+      <c r="T186" s="3">
         <v>-29.566666000000001</v>
       </c>
-      <c r="U173" s="3">
+      <c r="U186" s="3">
         <v>-50.250000999999997</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A174" s="3" t="s">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A187" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="B174" s="3" t="s">
+      <c r="B187" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="C187" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D187" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="E174" s="3" t="s">
+      <c r="E187" s="3" t="s">
         <v>853</v>
       </c>
-      <c r="F174" s="3" t="s">
+      <c r="F187" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="G174" s="3" t="s">
+      <c r="G187" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H174" s="3">
+      <c r="H187" s="3">
         <v>2011</v>
       </c>
-      <c r="I174" s="3">
+      <c r="I187" s="3">
         <v>9</v>
       </c>
-      <c r="J174" s="3">
+      <c r="J187" s="3">
         <v>3</v>
       </c>
-      <c r="K174" s="3">
+      <c r="K187" s="3">
         <v>278</v>
       </c>
-      <c r="L174" s="3">
+      <c r="L187" s="3">
         <v>288</v>
       </c>
-      <c r="O174" s="3" t="s">
+      <c r="O187" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="P174" s="8" t="s">
+      <c r="P187" s="8" t="s">
         <v>910</v>
       </c>
-      <c r="Q174" s="8" t="s">
+      <c r="Q187" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="R174" s="1" t="s">
+      <c r="R187" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S174" s="3" t="s">
+      <c r="S187" s="3" t="s">
         <v>909</v>
       </c>
-      <c r="T174" s="3">
+      <c r="T187" s="3">
         <v>-29.450008</v>
       </c>
-      <c r="U174" s="3">
+      <c r="U187" s="3">
         <v>-50.133341999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="3" t="s">
+    <row r="188" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="3" t="s">
         <v>856</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B188" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="C175" s="3" t="s">
+      <c r="C188" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="D175" s="3" t="s">
+      <c r="D188" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="E175" s="3" t="s">
+      <c r="E188" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="F175" s="3" t="s">
+      <c r="F188" s="3" t="s">
         <v>867</v>
       </c>
-      <c r="G175" s="3" t="s">
+      <c r="G188" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="H175" s="3">
+      <c r="H188" s="3">
         <f>2020</f>
         <v>2020</v>
       </c>
-      <c r="I175" s="3">
+      <c r="I188" s="3">
         <f>101</f>
         <v>101</v>
       </c>
-      <c r="J175" s="3">
+      <c r="J188" s="3">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="K175" s="3">
+      <c r="K188" s="3">
         <v>1561</v>
       </c>
-      <c r="L175" s="3">
+      <c r="L188" s="3">
         <v>1577</v>
       </c>
-      <c r="N175" s="3" t="s">
+      <c r="N188" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="O175" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="P175" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q175" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="R175" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="S175" s="3" t="s">
+      <c r="O188" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P188" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q188" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="R188" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="S188" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T175" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="U175" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A176" s="3" t="s">
+      <c r="T188" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="U188" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A189" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="B176" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="C176" s="3" t="s">
+      <c r="C189" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D176" s="3" t="s">
+      <c r="D189" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="E176" s="3" t="s">
+      <c r="E189" s="3" t="s">
         <v>863</v>
       </c>
-      <c r="F176" s="3" t="s">
+      <c r="F189" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="G176" s="3" t="s">
+      <c r="G189" s="3" t="s">
         <v>865</v>
       </c>
-      <c r="H176" s="12">
+      <c r="H189" s="12">
         <f>2021</f>
         <v>2021</v>
       </c>
-      <c r="I176" s="3">
+      <c r="I189" s="3">
         <f>155</f>
         <v>155</v>
       </c>
-      <c r="K176" s="12">
+      <c r="K189" s="12">
         <v>106992</v>
       </c>
-      <c r="N176" s="3" t="s">
+      <c r="N189" s="3" t="s">
         <v>887</v>
       </c>
-      <c r="O176" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="P176" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q176" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="R176" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="S176" s="3" t="s">
+      <c r="O189" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P189" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q189" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="R189" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="S189" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T176" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="U176" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A177" s="3" t="s">
+      <c r="T189" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="U189" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A190" s="3" t="s">
         <v>866</v>
       </c>
-      <c r="B177" s="12" t="s">
+      <c r="B190" s="12" t="s">
         <v>886</v>
       </c>
-      <c r="C177" s="12" t="s">
+      <c r="C190" s="12" t="s">
         <v>869</v>
       </c>
-      <c r="D177" s="10" t="s">
+      <c r="D190" s="10" t="s">
         <v>870</v>
       </c>
-      <c r="E177" s="13" t="s">
+      <c r="E190" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="F177" s="14" t="s">
+      <c r="F190" s="14" t="s">
         <v>871</v>
       </c>
-      <c r="G177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="H177" s="3">
+      <c r="G190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H190" s="3">
         <f>2016</f>
         <v>2016</v>
       </c>
-      <c r="I177" s="3">
+      <c r="I190" s="3">
         <f>25</f>
         <v>25</v>
       </c>
-      <c r="J177" s="3">
+      <c r="J190" s="3">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="K177" s="3">
+      <c r="K190" s="3">
         <f>92</f>
         <v>92</v>
       </c>
-      <c r="L177" s="3">
+      <c r="L190" s="3">
         <f>246</f>
         <v>246</v>
       </c>
-      <c r="O177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="P177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="R177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="S177" s="3" t="s">
+      <c r="O190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="R190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="S190" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T177" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="U177" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A178" s="3" t="s">
+      <c r="T190" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="U190" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A191" s="3" t="s">
         <v>868</v>
       </c>
-      <c r="B178" s="12" t="s">
+      <c r="B191" s="12" t="s">
         <v>872</v>
       </c>
-      <c r="C178" s="12" t="s">
+      <c r="C191" s="12" t="s">
         <v>872</v>
       </c>
-      <c r="D178" s="3" t="s">
+      <c r="D191" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="E178" s="3" t="s">
+      <c r="E191" s="3" t="s">
         <v>875</v>
       </c>
-      <c r="F178" s="15" t="s">
+      <c r="F191" s="15" t="s">
         <v>898</v>
       </c>
-      <c r="G178" s="3" t="s">
+      <c r="G191" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="H178" s="3">
+      <c r="H191" s="3">
         <f>2017</f>
         <v>2017</v>
       </c>
-      <c r="I178" s="3">
+      <c r="I191" s="3">
         <f>4294</f>
         <v>4294</v>
       </c>
-      <c r="J178" s="3">
+      <c r="J191" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K178" s="12">
+      <c r="K191" s="12">
         <v>71</v>
       </c>
-      <c r="L178" s="3">
+      <c r="L191" s="3">
         <f>92</f>
         <v>92</v>
       </c>
-      <c r="N178" s="11" t="s">
+      <c r="N191" s="11" t="s">
         <v>880</v>
       </c>
-      <c r="O178" s="3" t="s">
+      <c r="O191" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="P178" s="8" t="s">
+      <c r="P191" s="8" t="s">
         <v>930</v>
       </c>
-      <c r="Q178" s="8" t="s">
+      <c r="Q191" s="8" t="s">
         <v>931</v>
       </c>
-      <c r="R178" s="1" t="s">
+      <c r="R191" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="S178" s="3" t="s">
+      <c r="S191" s="3" t="s">
         <v>932</v>
       </c>
-      <c r="T178" s="3">
+      <c r="T191" s="3">
         <v>-29.48293</v>
       </c>
-      <c r="U178" s="3">
+      <c r="U191" s="3">
         <v>-50.205500000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A179" s="3" t="s">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A192" s="3" t="s">
         <v>873</v>
       </c>
-      <c r="B179" s="12" t="s">
+      <c r="B192" s="12" t="s">
         <v>879</v>
       </c>
-      <c r="C179" s="12" t="s">
+      <c r="C192" s="12" t="s">
         <v>879</v>
       </c>
-      <c r="D179" s="12" t="s">
+      <c r="D192" s="12" t="s">
         <v>899</v>
       </c>
-      <c r="E179" s="3" t="s">
+      <c r="E192" s="3" t="s">
         <v>875</v>
       </c>
-      <c r="F179" s="10" t="s">
+      <c r="F192" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="G179" s="3" t="s">
+      <c r="G192" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="H179" s="12">
+      <c r="H192" s="12">
         <f>2014</f>
         <v>2014</v>
       </c>
-      <c r="I179" s="12">
+      <c r="I192" s="12">
         <v>3811</v>
       </c>
-      <c r="K179" s="12">
+      <c r="K192" s="12">
         <v>207</v>
       </c>
-      <c r="L179" s="12">
+      <c r="L192" s="12">
         <v>225</v>
       </c>
-      <c r="N179" s="3" t="s">
+      <c r="N192" s="3" t="s">
         <v>880</v>
       </c>
-      <c r="O179" s="3" t="s">
+      <c r="O192" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="P179" s="8" t="s">
+      <c r="P192" s="8" t="s">
         <v>930</v>
       </c>
-      <c r="Q179" s="8" t="s">
+      <c r="Q192" s="8" t="s">
         <v>931</v>
       </c>
-      <c r="R179" s="1" t="s">
+      <c r="R192" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="S179" s="3" t="s">
+      <c r="S192" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="T179" s="3">
+      <c r="T192" s="3">
         <v>-29.48293</v>
       </c>
-      <c r="U179" s="3">
+      <c r="U192" s="3">
         <v>-50.205500000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A180" s="3" t="s">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A193" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="B180" s="12" t="s">
+      <c r="B193" s="12" t="s">
         <v>882</v>
       </c>
-      <c r="C180" s="12" t="s">
+      <c r="C193" s="12" t="s">
         <v>882</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D193" s="3" t="s">
         <v>881</v>
       </c>
-      <c r="E180" s="3" t="s">
+      <c r="E193" s="3" t="s">
         <v>877</v>
       </c>
-      <c r="F180" s="10" t="s">
+      <c r="F193" s="10" t="s">
         <v>883</v>
       </c>
-      <c r="G180" s="3" t="s">
+      <c r="G193" s="3" t="s">
         <v>884</v>
       </c>
-      <c r="H180" s="3">
+      <c r="H193" s="3">
         <f>2012</f>
         <v>2012</v>
       </c>
-      <c r="I180" s="3">
+      <c r="I193" s="3">
         <f>12</f>
         <v>12</v>
       </c>
-      <c r="J180" s="3">
+      <c r="J193" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K180" s="3">
+      <c r="K193" s="3">
         <f>261</f>
         <v>261</v>
       </c>
-      <c r="L180" s="3">
+      <c r="L193" s="3">
         <f>266</f>
         <v>266</v>
       </c>
-      <c r="N180" s="11" t="s">
+      <c r="N193" s="11" t="s">
         <v>885</v>
       </c>
-      <c r="O180" s="17" t="s">
+      <c r="O193" s="17" t="s">
         <v>934</v>
       </c>
-      <c r="P180" s="17" t="s">
+      <c r="P193" s="17" t="s">
         <v>935</v>
       </c>
-      <c r="Q180" s="17" t="s">
+      <c r="Q193" s="17" t="s">
         <v>936</v>
       </c>
-      <c r="R180" s="1" t="s">
+      <c r="R193" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="T180" s="3">
+      <c r="T193" s="3">
         <v>-32.116667</v>
       </c>
-      <c r="U180" s="3">
+      <c r="U193" s="3">
         <v>-52.15</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A181" s="3" t="s">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A194" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="B181" s="12" t="s">
+      <c r="B194" s="12" t="s">
         <v>882</v>
       </c>
-      <c r="C181" s="12" t="s">
+      <c r="C194" s="12" t="s">
         <v>882</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="D194" s="3" t="s">
         <v>881</v>
       </c>
-      <c r="E181" s="3" t="s">
+      <c r="E194" s="3" t="s">
         <v>877</v>
       </c>
-      <c r="F181" s="10" t="s">
+      <c r="F194" s="10" t="s">
         <v>883</v>
       </c>
-      <c r="G181" s="3" t="s">
+      <c r="G194" s="3" t="s">
         <v>884</v>
       </c>
-      <c r="H181" s="3">
+      <c r="H194" s="3">
         <f>2012</f>
         <v>2012</v>
       </c>
-      <c r="I181" s="3">
+      <c r="I194" s="3">
         <f>12</f>
         <v>12</v>
       </c>
-      <c r="J181" s="3">
+      <c r="J194" s="3">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K181" s="3">
+      <c r="K194" s="3">
         <f>261</f>
         <v>261</v>
       </c>
-      <c r="L181" s="3">
+      <c r="L194" s="3">
         <f>266</f>
         <v>266</v>
       </c>
-      <c r="N181" s="11" t="s">
+      <c r="N194" s="11" t="s">
         <v>885</v>
       </c>
-      <c r="O181" s="17" t="s">
+      <c r="O194" s="17" t="s">
         <v>937</v>
       </c>
-      <c r="P181" s="17" t="s">
+      <c r="P194" s="17" t="s">
         <v>938</v>
       </c>
-      <c r="Q181" s="17" t="s">
+      <c r="Q194" s="17" t="s">
         <v>939</v>
       </c>
-      <c r="R181" s="1" t="s">
+      <c r="R194" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="T181" s="3">
+      <c r="T194" s="3">
         <v>-32.15</v>
       </c>
-      <c r="U181" s="3">
+      <c r="U194" s="3">
         <v>-52.183332999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="3" t="s">
+    <row r="195" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
         <v>878</v>
       </c>
-      <c r="B182" s="12" t="s">
+      <c r="B195" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="C182" s="12" t="s">
+      <c r="C195" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="D182" s="16" t="s">
+      <c r="D195" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="E182" s="13" t="s">
+      <c r="E195" s="13" t="s">
         <v>901</v>
       </c>
-      <c r="F182" s="10" t="s">
+      <c r="F195" s="10" t="s">
         <v>889</v>
       </c>
-      <c r="G182" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="H182" s="12">
+      <c r="G195" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H195" s="12">
         <f>2014</f>
         <v>2014</v>
       </c>
-      <c r="I182" s="3">
+      <c r="I195" s="3">
         <f>10</f>
         <v>10</v>
       </c>
-      <c r="J182" s="3">
+      <c r="J195" s="3">
         <f>3</f>
         <v>3</v>
       </c>
-      <c r="K182" s="3">
+      <c r="K195" s="3">
         <f>650</f>
         <v>650</v>
       </c>
-      <c r="L182" s="3">
+      <c r="L195" s="3">
         <f>654</f>
         <v>654</v>
       </c>
-      <c r="N182" s="3" t="s">
+      <c r="N195" s="3" t="s">
         <v>890</v>
       </c>
-      <c r="O182" s="18" t="s">
+      <c r="O195" s="18" t="s">
         <v>940</v>
       </c>
-      <c r="P182" s="8" t="s">
+      <c r="P195" s="8" t="s">
         <v>941</v>
       </c>
-      <c r="Q182" s="8" t="s">
+      <c r="Q195" s="8" t="s">
         <v>942</v>
       </c>
-      <c r="R182" s="1" t="s">
+      <c r="R195" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="T182" s="3">
+      <c r="T195" s="3">
         <v>-30.011693000000001</v>
       </c>
-      <c r="U182" s="3">
+      <c r="U195" s="3">
         <v>-50.965049</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A183" s="3" t="s">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B183" s="12" t="s">
+      <c r="B196" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C183" s="12" t="s">
+      <c r="C196" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D196" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E183" s="13" t="s">
+      <c r="E196" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F183" s="16" t="s">
+      <c r="F196" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G183" s="3" t="s">
+      <c r="G196" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H183" s="3">
+      <c r="H196" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I183" s="3">
+      <c r="I196" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K183" s="3">
+      <c r="K196" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L183" s="3">
+      <c r="L196" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N183" s="11" t="s">
+      <c r="N196" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O183" s="3" t="s">
+      <c r="O196" s="3" t="s">
         <v>943</v>
       </c>
-      <c r="P183" s="19" t="s">
+      <c r="P196" s="19" t="s">
         <v>945</v>
       </c>
-      <c r="Q183" s="3" t="s">
+      <c r="Q196" s="3" t="s">
         <v>944</v>
       </c>
-      <c r="R183" s="1" t="s">
+      <c r="R196" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S183" s="3" t="s">
+      <c r="S196" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T183" s="3">
+      <c r="T196" s="3">
         <v>-28.05</v>
       </c>
-      <c r="U183" s="3">
+      <c r="U196" s="3">
         <v>-51.183332999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A184" s="3" t="s">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A197" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B184" s="12" t="s">
+      <c r="B197" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C184" s="12" t="s">
+      <c r="C197" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="D197" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E184" s="13" t="s">
+      <c r="E197" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F184" s="16" t="s">
+      <c r="F197" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G184" s="3" t="s">
+      <c r="G197" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H184" s="3">
+      <c r="H197" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I184" s="3">
+      <c r="I197" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K184" s="3">
+      <c r="K197" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L184" s="3">
+      <c r="L197" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N184" s="11" t="s">
+      <c r="N197" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O184" s="3" t="s">
+      <c r="O197" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="P184" s="19" t="s">
+      <c r="P197" s="19" t="s">
         <v>949</v>
       </c>
-      <c r="Q184" s="19" t="s">
+      <c r="Q197" s="19" t="s">
         <v>960</v>
       </c>
-      <c r="R184" s="1" t="s">
+      <c r="R197" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S184" s="3" t="s">
+      <c r="S197" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T184" s="3">
+      <c r="T197" s="3">
         <v>-29.316666999999999</v>
       </c>
-      <c r="U184" s="3">
+      <c r="U197" s="3">
         <v>-49.766666999999998</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A185" s="3" t="s">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B185" s="12" t="s">
+      <c r="B198" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C185" s="12" t="s">
+      <c r="C198" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D185" s="3" t="s">
+      <c r="D198" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E185" s="13" t="s">
+      <c r="E198" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F185" s="16" t="s">
+      <c r="F198" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G185" s="3" t="s">
+      <c r="G198" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H185" s="3">
+      <c r="H198" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I185" s="3">
+      <c r="I198" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K185" s="3">
+      <c r="K198" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L185" s="3">
+      <c r="L198" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N185" s="11" t="s">
+      <c r="N198" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O185" s="3" t="s">
+      <c r="O198" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="P185" s="19" t="s">
+      <c r="P198" s="19" t="s">
         <v>966</v>
       </c>
-      <c r="Q185" s="19" t="s">
+      <c r="Q198" s="19" t="s">
         <v>959</v>
       </c>
-      <c r="R185" s="1" t="s">
+      <c r="R198" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S185" s="3" t="s">
+      <c r="S198" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T185" s="3">
+      <c r="T198" s="3">
         <v>-29.883333</v>
       </c>
-      <c r="U185" s="3">
+      <c r="U198" s="3">
         <v>-50.266666000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A186" s="3" t="s">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A199" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B186" s="12" t="s">
+      <c r="B199" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C186" s="12" t="s">
+      <c r="C199" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D186" s="3" t="s">
+      <c r="D199" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E186" s="13" t="s">
+      <c r="E199" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F186" s="16" t="s">
+      <c r="F199" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G186" s="3" t="s">
+      <c r="G199" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H186" s="3">
+      <c r="H199" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I186" s="3">
+      <c r="I199" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K186" s="3">
+      <c r="K199" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L186" s="3">
+      <c r="L199" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N186" s="11" t="s">
+      <c r="N199" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O186" s="3" t="s">
+      <c r="O199" s="3" t="s">
         <v>946</v>
       </c>
-      <c r="P186" s="19" t="s">
+      <c r="P199" s="19" t="s">
         <v>950</v>
       </c>
-      <c r="Q186" s="19" t="s">
+      <c r="Q199" s="19" t="s">
         <v>959</v>
       </c>
-      <c r="R186" s="1" t="s">
+      <c r="R199" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S186" s="3" t="s">
+      <c r="S199" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T186" s="3">
+      <c r="T199" s="3">
         <v>-29.988502</v>
       </c>
-      <c r="U186" s="3">
+      <c r="U199" s="3">
         <v>-50.136975</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A187" s="3" t="s">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A200" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B187" s="12" t="s">
+      <c r="B200" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C187" s="12" t="s">
+      <c r="C200" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D187" s="3" t="s">
+      <c r="D200" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E187" s="13" t="s">
+      <c r="E200" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F187" s="16" t="s">
+      <c r="F200" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G187" s="3" t="s">
+      <c r="G200" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H187" s="3">
+      <c r="H200" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I187" s="3">
+      <c r="I200" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K187" s="3">
+      <c r="K200" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L187" s="3">
+      <c r="L200" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N187" s="11" t="s">
+      <c r="N200" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O187" s="3" t="s">
+      <c r="O200" s="3" t="s">
         <v>947</v>
       </c>
-      <c r="P187" s="19" t="s">
+      <c r="P200" s="19" t="s">
         <v>951</v>
       </c>
-      <c r="Q187" s="19" t="s">
+      <c r="Q200" s="19" t="s">
         <v>958</v>
       </c>
-      <c r="R187" s="1" t="s">
+      <c r="R200" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S187" s="3" t="s">
+      <c r="S200" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T187" s="3">
+      <c r="T200" s="3">
         <v>-29.95</v>
       </c>
-      <c r="U187" s="3">
+      <c r="U200" s="3">
         <v>-51.616667</v>
       </c>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A188" s="3" t="s">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A201" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B188" s="12" t="s">
+      <c r="B201" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C188" s="12" t="s">
+      <c r="C201" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D188" s="3" t="s">
+      <c r="D201" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E188" s="13" t="s">
+      <c r="E201" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F188" s="16" t="s">
+      <c r="F201" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G188" s="3" t="s">
+      <c r="G201" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H188" s="3">
+      <c r="H201" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I188" s="3">
+      <c r="I201" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K188" s="3">
+      <c r="K201" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L188" s="3">
+      <c r="L201" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N188" s="11" t="s">
+      <c r="N201" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O188" s="3" t="s">
+      <c r="O201" s="3" t="s">
         <v>948</v>
       </c>
-      <c r="P188" s="19" t="s">
+      <c r="P201" s="19" t="s">
         <v>952</v>
       </c>
-      <c r="Q188" s="19" t="s">
+      <c r="Q201" s="19" t="s">
         <v>957</v>
       </c>
-      <c r="R188" s="1" t="s">
+      <c r="R201" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S188" s="3" t="s">
+      <c r="S201" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T188" s="3">
+      <c r="T201" s="3">
         <v>-30.659524999999999</v>
       </c>
-      <c r="U188" s="3">
+      <c r="U201" s="3">
         <v>-51.394077000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A189" s="3" t="s">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A202" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B189" s="12" t="s">
+      <c r="B202" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C189" s="12" t="s">
+      <c r="C202" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D189" s="3" t="s">
+      <c r="D202" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E189" s="13" t="s">
+      <c r="E202" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F189" s="16" t="s">
+      <c r="F202" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G189" s="3" t="s">
+      <c r="G202" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H189" s="3">
+      <c r="H202" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I189" s="3">
+      <c r="I202" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K189" s="3">
+      <c r="K202" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L189" s="3">
+      <c r="L202" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N189" s="11" t="s">
+      <c r="N202" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O189" s="3" t="s">
+      <c r="O202" s="3" t="s">
         <v>922</v>
       </c>
-      <c r="P189" s="19" t="s">
+      <c r="P202" s="19" t="s">
         <v>953</v>
       </c>
-      <c r="Q189" s="19" t="s">
+      <c r="Q202" s="19" t="s">
         <v>956</v>
       </c>
-      <c r="R189" s="1" t="s">
+      <c r="R202" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S189" s="3" t="s">
+      <c r="S202" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T189" s="3">
+      <c r="T202" s="3">
         <v>-32.483333000000002</v>
       </c>
-      <c r="U189" s="3">
+      <c r="U202" s="3">
         <v>-52.566667000000002</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A190" s="3" t="s">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A203" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="B190" s="12" t="s">
+      <c r="B203" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="C190" s="12" t="s">
+      <c r="C203" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D203" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="E190" s="13" t="s">
+      <c r="E203" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="F190" s="16" t="s">
+      <c r="F203" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="G190" s="3" t="s">
+      <c r="G203" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H190" s="3">
+      <c r="H203" s="3">
         <f>2011</f>
         <v>2011</v>
       </c>
-      <c r="I190" s="3">
+      <c r="I203" s="3">
         <f>135</f>
         <v>135</v>
       </c>
-      <c r="K190" s="3">
+      <c r="K203" s="3">
         <f>126</f>
         <v>126</v>
       </c>
-      <c r="L190" s="3">
+      <c r="L203" s="3">
         <f>134</f>
         <v>134</v>
       </c>
-      <c r="N190" s="11" t="s">
+      <c r="N203" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="O190" s="3" t="s">
+      <c r="O203" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="P190" s="19" t="s">
+      <c r="P203" s="19" t="s">
         <v>954</v>
       </c>
-      <c r="Q190" s="19" t="s">
+      <c r="Q203" s="19" t="s">
         <v>955</v>
       </c>
-      <c r="R190" s="1" t="s">
+      <c r="R203" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="S190" s="3" t="s">
+      <c r="S203" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="T190" s="3">
+      <c r="T203" s="3">
         <v>-32.233342</v>
       </c>
-      <c r="U190" s="3">
+      <c r="U203" s="3">
         <v>-53.083314999999999</v>
       </c>
     </row>
@@ -16995,20 +17979,21 @@
     <hyperlink ref="N152" r:id="rId9" display="https://dx.doi.org/10.1002%2Fece3.1407" xr:uid="{D2268127-F515-47F2-BE78-A677B1D72FBF}"/>
     <hyperlink ref="N153" r:id="rId10" display="https://dx.doi.org/10.1002%2Fece3.1407" xr:uid="{7648F2DF-7DBB-4170-A27B-24832BD859EE}"/>
     <hyperlink ref="N154" r:id="rId11" display="https://dx.doi.org/10.1002%2Fece3.1407" xr:uid="{9D105C02-CB82-4711-9441-A6289DFE24F0}"/>
-    <hyperlink ref="N178" r:id="rId12" display="https://doi.org/10.11646/zootaxa.4294.1.3" xr:uid="{18456167-071A-4EDB-A698-E78F4189F3DE}"/>
-    <hyperlink ref="N180" r:id="rId13" display="https://doi.org/10.1590/S1676-06032012000100021" xr:uid="{7582FE18-B114-42DB-9FF5-F0C92946619B}"/>
-    <hyperlink ref="N183" r:id="rId14" display="https://doi.org/10.1159/000331584" xr:uid="{4DFA5952-5C76-4ACB-8515-3977CF67D0AF}"/>
-    <hyperlink ref="N181" r:id="rId15" display="https://doi.org/10.1590/S1676-06032012000100021" xr:uid="{B90FB598-F298-4D38-8203-C64822BA50D6}"/>
-    <hyperlink ref="N184" r:id="rId16" display="https://doi.org/10.1159/000331584" xr:uid="{EE1C2CBD-D97D-418E-AF17-784218513E13}"/>
-    <hyperlink ref="N185" r:id="rId17" display="https://doi.org/10.1159/000331584" xr:uid="{744F3292-CCDB-4E9A-B1BB-EF0FD6B01E18}"/>
-    <hyperlink ref="N186" r:id="rId18" display="https://doi.org/10.1159/000331584" xr:uid="{6584E2E9-314E-421B-8044-8A17FE6ED221}"/>
-    <hyperlink ref="N187" r:id="rId19" display="https://doi.org/10.1159/000331584" xr:uid="{E55A6105-68BB-4CEA-89A8-80FF64A71B18}"/>
-    <hyperlink ref="N188" r:id="rId20" display="https://doi.org/10.1159/000331584" xr:uid="{85ECB3B9-6817-4244-879B-38AB39F7CE9E}"/>
-    <hyperlink ref="N189" r:id="rId21" display="https://doi.org/10.1159/000331584" xr:uid="{FBC504F2-C4E0-4929-8701-813509AA7306}"/>
-    <hyperlink ref="N190" r:id="rId22" display="https://doi.org/10.1159/000331584" xr:uid="{D3B8D442-4FCD-4FFD-B557-42DF7F91B421}"/>
+    <hyperlink ref="N191" r:id="rId12" display="https://doi.org/10.11646/zootaxa.4294.1.3" xr:uid="{18456167-071A-4EDB-A698-E78F4189F3DE}"/>
+    <hyperlink ref="N193" r:id="rId13" display="https://doi.org/10.1590/S1676-06032012000100021" xr:uid="{7582FE18-B114-42DB-9FF5-F0C92946619B}"/>
+    <hyperlink ref="N196" r:id="rId14" display="https://doi.org/10.1159/000331584" xr:uid="{4DFA5952-5C76-4ACB-8515-3977CF67D0AF}"/>
+    <hyperlink ref="N194" r:id="rId15" display="https://doi.org/10.1590/S1676-06032012000100021" xr:uid="{B90FB598-F298-4D38-8203-C64822BA50D6}"/>
+    <hyperlink ref="N197" r:id="rId16" display="https://doi.org/10.1159/000331584" xr:uid="{EE1C2CBD-D97D-418E-AF17-784218513E13}"/>
+    <hyperlink ref="N198" r:id="rId17" display="https://doi.org/10.1159/000331584" xr:uid="{744F3292-CCDB-4E9A-B1BB-EF0FD6B01E18}"/>
+    <hyperlink ref="N199" r:id="rId18" display="https://doi.org/10.1159/000331584" xr:uid="{6584E2E9-314E-421B-8044-8A17FE6ED221}"/>
+    <hyperlink ref="N200" r:id="rId19" display="https://doi.org/10.1159/000331584" xr:uid="{E55A6105-68BB-4CEA-89A8-80FF64A71B18}"/>
+    <hyperlink ref="N201" r:id="rId20" display="https://doi.org/10.1159/000331584" xr:uid="{85ECB3B9-6817-4244-879B-38AB39F7CE9E}"/>
+    <hyperlink ref="N202" r:id="rId21" display="https://doi.org/10.1159/000331584" xr:uid="{FBC504F2-C4E0-4929-8701-813509AA7306}"/>
+    <hyperlink ref="N203" r:id="rId22" display="https://doi.org/10.1159/000331584" xr:uid="{D3B8D442-4FCD-4FFD-B557-42DF7F91B421}"/>
+    <hyperlink ref="N168" r:id="rId23" display="https://doi.org/10.1590/S1676-06032008000100015" xr:uid="{317B3B09-B983-4EBE-ADF3-B007E0C74F9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update data, figs, results
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chapter_overbeck\mammals_book\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEC2B05-4441-4123-A3B5-E36C5D30008B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38252633-7905-4C35-9951-8247D62ADB33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">search!$A$1:$U$318</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">search!$A$1:$AA$318</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="1568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="1567">
   <si>
     <t>Authors</t>
   </si>
@@ -4782,9 +4782,6 @@
   </si>
   <si>
     <t>Non-flying small mammals</t>
-  </si>
-  <si>
-    <t>Small mammals</t>
   </si>
   <si>
     <t>Notoungulata</t>
@@ -5357,10 +5354,10 @@
   <dimension ref="A1:AA318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C282" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A317" sqref="A317"/>
+      <selection pane="bottomRight" activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6975,7 +6972,7 @@
         <v>507</v>
       </c>
       <c r="V22" s="32" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
@@ -7048,7 +7045,7 @@
         <v>507</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
@@ -10183,7 +10180,7 @@
         <v>-50.106586</v>
       </c>
       <c r="V66" s="7" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="W66" s="7"/>
       <c r="X66" s="7"/>
@@ -10475,7 +10472,7 @@
         <v>507</v>
       </c>
       <c r="V70" s="8" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="71" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
@@ -10689,7 +10686,7 @@
         <v>-55.384999999999998</v>
       </c>
       <c r="V73" s="31" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="W73" s="7"/>
       <c r="X73" s="7"/>
@@ -12066,7 +12063,7 @@
         <v>507</v>
       </c>
       <c r="V92" s="7" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="W92" s="7"/>
       <c r="X92" s="7"/>
@@ -12139,7 +12136,7 @@
         <v>507</v>
       </c>
       <c r="V93" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W93" s="7"/>
       <c r="X93" s="7"/>
@@ -12859,7 +12856,7 @@
         <v>-50.216786999999997</v>
       </c>
       <c r="V103" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W103" s="7"/>
       <c r="X103" s="7"/>
@@ -12932,7 +12929,7 @@
         <v>-51.678320999999997</v>
       </c>
       <c r="V104" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W104" s="7"/>
       <c r="X104" s="7"/>
@@ -13297,7 +13294,7 @@
         <v>507</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="W109" s="7"/>
       <c r="X109" s="7"/>
@@ -13370,7 +13367,7 @@
         <v>507</v>
       </c>
       <c r="V110" s="32" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="W110" s="7"/>
       <c r="X110" s="7"/>
@@ -13516,7 +13513,7 @@
         <v>-54.837803999999998</v>
       </c>
       <c r="V112" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W112" s="7"/>
       <c r="X112" s="7"/>
@@ -13589,7 +13586,7 @@
         <v>-54.766126999999997</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="114" spans="1:27" ht="15.75" x14ac:dyDescent="0.2">
@@ -13657,7 +13654,7 @@
         <v>507</v>
       </c>
       <c r="V114" s="32" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="115" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
@@ -13871,7 +13868,7 @@
         <v>507</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="W117" s="7"/>
       <c r="X117" s="7"/>
@@ -13944,7 +13941,7 @@
         <v>507</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="W118" s="7"/>
       <c r="X118" s="7"/>
@@ -15331,7 +15328,7 @@
         <v>507</v>
       </c>
       <c r="V137" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="W137" s="7"/>
       <c r="X137" s="7"/>
@@ -15550,7 +15547,7 @@
         <v>507</v>
       </c>
       <c r="V140" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="W140" s="7"/>
       <c r="X140" s="7"/>
@@ -15844,7 +15841,7 @@
         <v>-51.604446000000003</v>
       </c>
       <c r="V144" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W144" s="7"/>
       <c r="X144" s="7"/>
@@ -15920,7 +15917,7 @@
         <v>-51.053435</v>
       </c>
       <c r="V145" s="7" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W145" s="7"/>
       <c r="X145" s="7"/>
@@ -17597,7 +17594,7 @@
         <v>-53.715730000000001</v>
       </c>
       <c r="V168" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="169" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -17959,7 +17956,7 @@
         <v>-51.671531000000002</v>
       </c>
       <c r="V173" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="174" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -18030,7 +18027,7 @@
         <v>-51.712150999999999</v>
       </c>
       <c r="V174" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="175" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -18711,7 +18708,7 @@
         <v>-50.383333</v>
       </c>
       <c r="V184" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="185" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -18779,7 +18776,7 @@
         <v>-50.416646</v>
       </c>
       <c r="V185" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="186" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -18847,7 +18844,7 @@
         <v>-50.250000999999997</v>
       </c>
       <c r="V186" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="187" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -18915,7 +18912,7 @@
         <v>-50.133341999999999</v>
       </c>
       <c r="V187" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="188" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -19129,7 +19126,7 @@
         <v>507</v>
       </c>
       <c r="V190" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="191" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -19343,7 +19340,7 @@
         <v>-52.15</v>
       </c>
       <c r="V193" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="194" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -19416,7 +19413,7 @@
         <v>-52.183332999999998</v>
       </c>
       <c r="V194" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="195" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -22929,7 +22926,7 @@
         <v>-51.966667999999999</v>
       </c>
       <c r="V244" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="245" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23065,7 +23062,7 @@
         <v>-50.249904999999998</v>
       </c>
       <c r="V246" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="247" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23133,7 +23130,7 @@
         <v>-49.157138000000003</v>
       </c>
       <c r="V247" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="248" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23269,7 +23266,7 @@
         <v>-49.666666999999997</v>
       </c>
       <c r="V249" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="250" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23337,7 +23334,7 @@
         <v>-48.816667000000002</v>
       </c>
       <c r="V250" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="251" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23405,7 +23402,7 @@
         <v>-48.816667000000002</v>
       </c>
       <c r="V251" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="252" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23473,7 +23470,7 @@
         <v>-48.85</v>
       </c>
       <c r="V252" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="253" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23541,7 +23538,7 @@
         <v>-48.430833</v>
       </c>
       <c r="V253" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="254" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23609,7 +23606,7 @@
         <v>-51.1218</v>
       </c>
       <c r="V254" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="255" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23681,7 +23678,7 @@
         <v>-52.418157999999998</v>
       </c>
       <c r="V255" s="8" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="256" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23753,7 +23750,7 @@
         <v>-50.000556000000003</v>
       </c>
       <c r="V256" s="8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="257" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23825,7 +23822,7 @@
         <v>-50.00611</v>
       </c>
       <c r="V257" s="8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="258" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23898,7 +23895,7 @@
         <v>-49.766666999999998</v>
       </c>
       <c r="V258" s="8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="259" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -23971,7 +23968,7 @@
         <v>-49.816667000000002</v>
       </c>
       <c r="V259" s="8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="260" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -28179,7 +28176,7 @@
         <v>-50.383333</v>
       </c>
       <c r="V317" s="8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="318" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -28256,7 +28253,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U318" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AA318" xr:uid="{4395F58A-E2C9-4E5B-B63D-3F65004A485F}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N143" r:id="rId1" display="https://doi.org/10.1590/S1984-46702010000100015" xr:uid="{491E9D6D-3641-410F-8F78-C99777E23581}"/>

</xml_diff>